<commit_message>
DEV 14 - Final Fix
</commit_message>
<xml_diff>
--- a/resources/data/ManagerList.xlsx
+++ b/resources/data/ManagerList.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a02774ed8d28bca/Desktop/NTU/NTU_Y1S2/SC2002/Assignment/BTO_Application/files/"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -56,12 +56,16 @@
   </si>
   <si>
     <t>Married</t>
+  </si>
+  <si>
+    <t>npassword</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -953,7 +957,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">

</xml_diff>